<commit_message>
a billion excel/csv files
</commit_message>
<xml_diff>
--- a/data/Preferences_wsheets.xlsx
+++ b/data/Preferences_wsheets.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PyCharm\DFTMapping\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\PycharmProjects\DFTMapping\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{63767503-C8BF-4E04-8BDB-D6AF70205C2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA4A3A49-1911-4489-97C6-8FEE03BD27AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" firstSheet="2" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-2604" yWindow="3276" windowWidth="5760" windowHeight="2484" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="NI" sheetId="12" r:id="rId1"/>
@@ -7177,7 +7177,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40667BD3-E9B4-40F9-B232-4EC72B093E86}">
   <dimension ref="A1:N114"/>
   <sheetViews>
-    <sheetView topLeftCell="A76" workbookViewId="0">
+    <sheetView topLeftCell="A26" workbookViewId="0">
       <selection activeCell="G56" sqref="G56"/>
     </sheetView>
   </sheetViews>
@@ -11442,8 +11442,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B063618-9A6D-4A91-ADD8-3B03FB31A1AE}">
   <dimension ref="A1:N80"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A71" sqref="A71"/>
+    <sheetView topLeftCell="A3" zoomScale="82" zoomScaleNormal="82" workbookViewId="0">
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -14336,8 +14336,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E2A68F8-2243-4733-8543-8E0D41F4BD01}">
   <dimension ref="A1:N47"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K38" sqref="K38"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -16157,7 +16157,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3593190B-54A6-41F5-9BBB-1B886F4B4A9E}">
   <dimension ref="A1:N69"/>
   <sheetViews>
-    <sheetView topLeftCell="A55" workbookViewId="0">
+    <sheetView topLeftCell="A11" workbookViewId="0">
       <selection sqref="A1:N1"/>
     </sheetView>
   </sheetViews>
@@ -21707,13 +21707,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N69"/>
   <sheetViews>
-    <sheetView topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="A54" sqref="A54"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
+      <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="78.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33.44140625" customWidth="1"/>
     <col min="3" max="3" width="15.6640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="8.33203125" customWidth="1"/>
     <col min="7" max="7" width="40.88671875" customWidth="1"/>
@@ -24282,7 +24282,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42CFF303-42F7-4252-8916-74CFFBB125B3}">
   <dimension ref="A1:N91"/>
   <sheetViews>
-    <sheetView topLeftCell="A70" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K53" sqref="K53"/>
     </sheetView>
   </sheetViews>
@@ -27705,18 +27705,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{184DA011-67BE-4D91-A899-197331CA684E}">
   <dimension ref="A1:N91"/>
   <sheetViews>
-    <sheetView topLeftCell="E19" workbookViewId="0">
-      <selection activeCell="K38" sqref="K38"/>
+    <sheetView topLeftCell="A21" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="K63" sqref="K63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="19.21875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="49.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.77734375" customWidth="1"/>
     <col min="3" max="3" width="15.6640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11.109375" customWidth="1"/>
-    <col min="9" max="9" width="11.6640625" customWidth="1"/>
-    <col min="10" max="10" width="13.88671875" customWidth="1"/>
+    <col min="8" max="8" width="5.33203125" customWidth="1"/>
+    <col min="9" max="9" width="2.77734375" customWidth="1"/>
+    <col min="10" max="10" width="2.6640625" customWidth="1"/>
     <col min="11" max="11" width="146.6640625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="15.6640625" customWidth="1"/>
     <col min="13" max="13" width="17.44140625" customWidth="1"/>
@@ -30926,8 +30927,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{131CA9D3-CA9E-42F6-A903-E6D3B2CB0C36}">
   <dimension ref="A1:O47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="L21" sqref="L21"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -32793,7 +32794,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11DF21C6-CA39-4492-9B4C-0FF8BE65D31F}">
   <dimension ref="A1:N95"/>
   <sheetViews>
-    <sheetView topLeftCell="A40" workbookViewId="0">
+    <sheetView topLeftCell="B1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
@@ -32801,12 +32802,12 @@
   <cols>
     <col min="1" max="1" width="19.21875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.77734375" customWidth="1"/>
-    <col min="3" max="3" width="17" customWidth="1"/>
+    <col min="3" max="3" width="2.6640625" customWidth="1"/>
     <col min="6" max="6" width="7.6640625" customWidth="1"/>
     <col min="7" max="7" width="10.5546875" customWidth="1"/>
-    <col min="8" max="8" width="11.109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="21.77734375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.109375" customWidth="1"/>
+    <col min="9" max="9" width="4" customWidth="1"/>
+    <col min="10" max="10" width="3.44140625" customWidth="1"/>
     <col min="11" max="11" width="137.5546875" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="13.5546875" bestFit="1" customWidth="1"/>
   </cols>
@@ -36359,8 +36360,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E75A2F8B-EC80-4EEF-87C3-785B8330CC0D}">
   <dimension ref="A1:N48"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="L19" sqref="L19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>